<commit_message>
updates for inflow depth
</commit_message>
<xml_diff>
--- a/bathymetry/bath_map.xlsx
+++ b/bathymetry/bath_map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rqthomas/Documents/research/global-centers/elcom-dev/AED_Tools_Private/FCR_ELCOM_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rqthomas/Documents/research/global-centers/ELCOM_FCR/bathymetry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB5F3D87-E5F4-B144-9A44-A3861C3A1CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC164BD4-447C-504E-B9FC-92924A8445E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="2140" windowWidth="26840" windowHeight="15940" xr2:uid="{21BF40BF-23D7-724C-A6E3-7D70C9DA760D}"/>
+    <workbookView xWindow="2840" yWindow="5240" windowWidth="26840" windowHeight="15940" xr2:uid="{21BF40BF-23D7-724C-A6E3-7D70C9DA760D}"/>
   </bookViews>
   <sheets>
     <sheet name="bath" sheetId="1" r:id="rId1"/>
@@ -536,11 +536,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -921,93 +920,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29EA120-A3A2-AC45-ABF3-1965E8BB511B}">
   <dimension ref="A1:AE74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="26" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="3">
         <v>6</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="3">
         <v>7</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="3">
         <v>8</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="3">
         <v>9</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="3">
         <v>10</v>
       </c>
-      <c r="L1" s="4">
+      <c r="L1" s="3">
         <v>11</v>
       </c>
-      <c r="M1" s="4">
+      <c r="M1" s="3">
         <v>12</v>
       </c>
-      <c r="N1" s="4">
+      <c r="N1" s="3">
         <v>13</v>
       </c>
-      <c r="O1" s="4">
+      <c r="O1" s="3">
         <v>14</v>
       </c>
-      <c r="P1" s="4">
+      <c r="P1" s="3">
         <v>15</v>
       </c>
-      <c r="Q1" s="4">
+      <c r="Q1" s="3">
         <v>16</v>
       </c>
-      <c r="R1" s="4">
+      <c r="R1" s="3">
         <v>17</v>
       </c>
-      <c r="S1" s="4">
+      <c r="S1" s="3">
         <v>18</v>
       </c>
-      <c r="T1" s="4">
+      <c r="T1" s="3">
         <v>19</v>
       </c>
-      <c r="U1" s="4">
+      <c r="U1" s="3">
         <v>20</v>
       </c>
-      <c r="V1" s="4">
+      <c r="V1" s="3">
         <v>21</v>
       </c>
-      <c r="W1" s="4">
+      <c r="W1" s="3">
         <v>22</v>
       </c>
-      <c r="X1" s="4">
+      <c r="X1" s="3">
         <v>23</v>
       </c>
-      <c r="Y1" s="4">
+      <c r="Y1" s="3">
         <v>24</v>
       </c>
-      <c r="Z1" s="4">
+      <c r="Z1" s="3">
         <v>25</v>
       </c>
       <c r="AD1" t="s">
@@ -1015,7 +1014,7 @@
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -1101,7 +1100,7 @@
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -1187,7 +1186,7 @@
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -1273,7 +1272,7 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -1359,7 +1358,7 @@
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -1445,7 +1444,7 @@
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -1531,7 +1530,7 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -1617,7 +1616,7 @@
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="1">
@@ -1703,7 +1702,7 @@
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -1789,7 +1788,7 @@
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -1875,7 +1874,7 @@
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="1">
@@ -1961,7 +1960,7 @@
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="1">
@@ -2047,7 +2046,7 @@
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="1">
@@ -2133,7 +2132,7 @@
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="1">
@@ -2219,7 +2218,7 @@
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="1">
@@ -2305,7 +2304,7 @@
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="1">
@@ -2391,7 +2390,7 @@
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="1">
@@ -2477,7 +2476,7 @@
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="1">
@@ -2563,7 +2562,7 @@
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="1">
@@ -2649,7 +2648,7 @@
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="1">
@@ -2715,8 +2714,8 @@
       <c r="V21" s="1">
         <v>-1.18446511627907</v>
       </c>
-      <c r="W21" s="5">
-        <v>-0.22572043010752699</v>
+      <c r="W21" s="4">
+        <v>-1</v>
       </c>
       <c r="X21" s="1">
         <v>999.9</v>
@@ -2735,7 +2734,7 @@
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="1">
@@ -2802,7 +2801,7 @@
         <v>-1.18446511627907</v>
       </c>
       <c r="W22" s="1">
-        <v>-0.53409090909090895</v>
+        <v>-1</v>
       </c>
       <c r="X22" s="1">
         <v>999.9</v>
@@ -2821,7 +2820,7 @@
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="1">
@@ -2888,7 +2887,7 @@
         <v>-1.6967938931297699</v>
       </c>
       <c r="W23" s="1">
-        <v>-0.53409090909090895</v>
+        <v>-1</v>
       </c>
       <c r="X23" s="1">
         <v>999.9</v>
@@ -2907,7 +2906,7 @@
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="1">
@@ -2993,7 +2992,7 @@
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="1">
@@ -3079,7 +3078,7 @@
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="1">
@@ -3165,7 +3164,7 @@
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="1">
@@ -3251,7 +3250,7 @@
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="1">
@@ -3337,7 +3336,7 @@
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="1">
@@ -3423,7 +3422,7 @@
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="1">
@@ -3509,7 +3508,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="1">
@@ -3542,7 +3541,7 @@
       <c r="K31" s="2">
         <v>-3.9497530864197499</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="1">
         <v>-4.2197500000000003</v>
       </c>
       <c r="M31" s="1">
@@ -3595,7 +3594,7 @@
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="1">
@@ -3681,7 +3680,7 @@
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="1">
@@ -3767,7 +3766,7 @@
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="1">
@@ -3853,7 +3852,7 @@
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="1">
@@ -3939,7 +3938,7 @@
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="1">
@@ -4025,7 +4024,7 @@
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="1">
@@ -4111,7 +4110,7 @@
       </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="1">
@@ -4197,7 +4196,7 @@
       </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="1">
@@ -4283,7 +4282,7 @@
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="1">
@@ -4310,7 +4309,7 @@
       <c r="I40" s="2">
         <v>-5.0691428571428601</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="1">
         <v>-5.2138461538461502</v>
       </c>
       <c r="K40" s="1">
@@ -4369,7 +4368,7 @@
       </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="1">
@@ -4455,7 +4454,7 @@
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="1">
@@ -4541,7 +4540,7 @@
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="1">
@@ -4627,7 +4626,7 @@
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="1">
@@ -4651,7 +4650,7 @@
       <c r="H44" s="2">
         <v>-5.6755000000000004</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="1">
         <v>-5.84</v>
       </c>
       <c r="J44" s="1">
@@ -4713,7 +4712,7 @@
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" s="1">
@@ -4799,7 +4798,7 @@
       </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" s="1">
@@ -4885,7 +4884,7 @@
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" s="1">
@@ -4971,7 +4970,7 @@
       </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="1">
@@ -4992,7 +4991,7 @@
       <c r="G48" s="2">
         <v>-5.7968421052631598</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="1">
         <v>-6.2567857142857104</v>
       </c>
       <c r="I48" s="1">
@@ -5057,7 +5056,7 @@
       </c>
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" s="1">
@@ -5143,7 +5142,7 @@
       </c>
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="1">
@@ -5229,7 +5228,7 @@
       </c>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" s="1">
@@ -5315,7 +5314,7 @@
       </c>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
       <c r="B52" s="1">
@@ -5401,7 +5400,7 @@
       </c>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" s="1">
@@ -5487,7 +5486,7 @@
       </c>
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
       <c r="B54" s="1">
@@ -5573,7 +5572,7 @@
       </c>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>54</v>
       </c>
       <c r="B55" s="1">
@@ -5659,7 +5658,7 @@
       </c>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" s="1">
@@ -5745,7 +5744,7 @@
       </c>
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>56</v>
       </c>
       <c r="B57" s="1">
@@ -5831,7 +5830,7 @@
       </c>
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
       <c r="B58" s="1">
@@ -5917,7 +5916,7 @@
       </c>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A59" s="4">
+      <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" s="1">
@@ -6003,7 +6002,7 @@
       </c>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>59</v>
       </c>
       <c r="B60" s="1">
@@ -6024,7 +6023,7 @@
       <c r="G60" s="1">
         <v>-5.0444827586206902</v>
       </c>
-      <c r="H60" s="3">
+      <c r="H60" s="1">
         <v>-6.1323809523809496</v>
       </c>
       <c r="I60" s="2">
@@ -6089,7 +6088,7 @@
       </c>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A61" s="4">
+      <c r="A61" s="3">
         <v>60</v>
       </c>
       <c r="B61" s="1">
@@ -6113,7 +6112,7 @@
       <c r="H61" s="1">
         <v>-6.1323809523809496</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61" s="1">
         <v>-7.0722857142857096</v>
       </c>
       <c r="J61" s="2">
@@ -6175,7 +6174,7 @@
       </c>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" s="1">
@@ -6202,7 +6201,7 @@
       <c r="I62" s="1">
         <v>-7.4715909090909101</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J62" s="1">
         <v>-8.3883544303797493</v>
       </c>
       <c r="K62" s="2">
@@ -6261,7 +6260,7 @@
       </c>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A63" s="4">
+      <c r="A63" s="3">
         <v>62</v>
       </c>
       <c r="B63" s="1">
@@ -6291,7 +6290,7 @@
       <c r="J63" s="1">
         <v>-8.5311711711711702</v>
       </c>
-      <c r="K63" s="3">
+      <c r="K63" s="1">
         <v>-8.6147727272727295</v>
       </c>
       <c r="L63" s="2">
@@ -6347,7 +6346,7 @@
       </c>
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A64" s="4">
+      <c r="A64" s="3">
         <v>63</v>
       </c>
       <c r="B64" s="1">
@@ -6380,7 +6379,7 @@
       <c r="K64" s="1">
         <v>-8.7770491803278698</v>
       </c>
-      <c r="L64" s="3">
+      <c r="L64" s="1">
         <v>-8.8797674418604693</v>
       </c>
       <c r="M64" s="2">
@@ -6433,7 +6432,7 @@
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A65" s="4">
+      <c r="A65" s="3">
         <v>64</v>
       </c>
       <c r="B65" s="1">
@@ -6469,7 +6468,7 @@
       <c r="L65" s="1">
         <v>-8.9585454545454493</v>
       </c>
-      <c r="M65" s="3">
+      <c r="M65" s="1">
         <v>-9.4471428571428593</v>
       </c>
       <c r="N65" s="2">
@@ -6519,7 +6518,7 @@
       </c>
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A66" s="4">
+      <c r="A66" s="3">
         <v>65</v>
       </c>
       <c r="B66" s="1">
@@ -6558,7 +6557,7 @@
       <c r="M66" s="1">
         <v>-9.2569930069930102</v>
       </c>
-      <c r="N66" s="3">
+      <c r="N66" s="1">
         <v>-9.2570886075949392</v>
       </c>
       <c r="O66" s="2">
@@ -6605,7 +6604,7 @@
       </c>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A67" s="4">
+      <c r="A67" s="3">
         <v>66</v>
       </c>
       <c r="B67" s="1">
@@ -6647,7 +6646,7 @@
       <c r="N67" s="1">
         <v>-9.1639999999999997</v>
       </c>
-      <c r="O67" s="3">
+      <c r="O67" s="1">
         <v>-9.3468586387434591</v>
       </c>
       <c r="P67" s="2">
@@ -6691,7 +6690,7 @@
       </c>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A68" s="4">
+      <c r="A68" s="3">
         <v>67</v>
       </c>
       <c r="B68" s="1">
@@ -6777,7 +6776,7 @@
       </c>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A69" s="4">
+      <c r="A69" s="3">
         <v>68</v>
       </c>
       <c r="B69" s="1">
@@ -6863,7 +6862,7 @@
       </c>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A70" s="4">
+      <c r="A70" s="3">
         <v>69</v>
       </c>
       <c r="B70" s="1">
@@ -6949,7 +6948,7 @@
       </c>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A71" s="4">
+      <c r="A71" s="3">
         <v>70</v>
       </c>
       <c r="B71" s="1">
@@ -7003,7 +7002,7 @@
       <c r="R71" s="1">
         <v>-9.9865254237288106</v>
       </c>
-      <c r="S71" s="3">
+      <c r="S71" s="1">
         <v>-10.0286111111111</v>
       </c>
       <c r="T71" s="1">
@@ -7035,7 +7034,7 @@
       </c>
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A72" s="4">
+      <c r="A72" s="3">
         <v>71</v>
       </c>
       <c r="B72" s="1">
@@ -7121,7 +7120,7 @@
       </c>
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A73" s="4">
+      <c r="A73" s="3">
         <v>72</v>
       </c>
       <c r="B73" s="1">
@@ -7157,7 +7156,7 @@
       <c r="L73" s="1">
         <v>-1.8281825657894699</v>
       </c>
-      <c r="M73" s="6">
+      <c r="M73" s="5">
         <v>-1.7953125000000001</v>
       </c>
       <c r="N73" s="1">
@@ -7207,7 +7206,7 @@
       </c>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A74" s="4">
+      <c r="A74" s="3">
         <v>73</v>
       </c>
       <c r="B74" s="1">

</xml_diff>